<commit_message>
Update NB3 Body PCB (rev 6)
</commit_message>
<xml_diff>
--- a/boxes/electrons/NB3_body/fab/NB3_body.xlsx
+++ b/boxes/electrons/NB3_body/fab/NB3_body.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="NB3_power" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NB3_power" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -49,18 +49,21 @@
     <t xml:space="preserve">J12,J13</t>
   </si>
   <si>
-    <t xml:space="preserve">Male Header 2x03 Surface Mount 2.54mm SMD P=2.54mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ckmtw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C124390</t>
+    <t xml:space="preserve">Male Header 2x03 Through-Hole 2.54mm P=2.54mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XFCN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PZ254V-12-6P</t>
   </si>
   <si>
     <t xml:space="preserve">LCSC</t>
   </si>
   <si>
+    <t xml:space="preserve">C492420</t>
+  </si>
+  <si>
     <t xml:space="preserve">J1,J2,J4,J15,J3,J5,J14,J6</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">BOOMELE</t>
   </si>
   <si>
+    <t xml:space="preserve">2.54-2*5P</t>
+  </si>
+  <si>
     <t xml:space="preserve">C261072</t>
   </si>
   <si>
@@ -79,10 +85,13 @@
     <t xml:space="preserve">Female Header 2x07 Surface Mount 2.54mm SMD P=2.54mm</t>
   </si>
   <si>
+    <t xml:space="preserve">2.54-2*7P</t>
+  </si>
+  <si>
     <t xml:space="preserve">C84005</t>
   </si>
   <si>
-    <t xml:space="preserve">J10</t>
+    <t xml:space="preserve">J11,J10</t>
   </si>
   <si>
     <t xml:space="preserve">PH Header Male Pin 0.079"(2.00mm) 4 SMD P=2mm Wire To Board / Wire To Wire </t>
@@ -305,6 +314,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -313,7 +428,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -376,10 +491,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="n">
-        <v>0.05</v>
+        <v>0.0354</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -387,22 +502,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0.1428</v>
@@ -413,22 +528,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0.2098</v>
@@ -436,25 +551,25 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0.2873</v>
@@ -472,7 +587,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H9" s="5"/>
     </row>

</xml_diff>